<commit_message>
schema updated in db
</commit_message>
<xml_diff>
--- a/images/permissions.xlsx
+++ b/images/permissions.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9180dbd63a053c90/Desktop/GitHub/FamilyTraditions/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="11_F25DC773A252ABDACC1048C3395A4B325ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A9A22F7-9AA1-435D-905A-348825F70558}"/>
+  <xr:revisionPtr revIDLastSave="103" documentId="11_F25DC773A252ABDACC1048C3395A4B325ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A6C2B932-6456-4539-A8AA-3EE369A244E7}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recipe_Book_Permissions" sheetId="1" r:id="rId1"/>
+    <sheet name="Test Accounts" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
   <si>
     <t>Create Recipe</t>
   </si>
@@ -55,13 +56,115 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Test_User_1</t>
+  </si>
+  <si>
+    <t>Test_User_2</t>
+  </si>
+  <si>
+    <t>Test_User_3</t>
+  </si>
+  <si>
+    <t>Test_User_4</t>
+  </si>
+  <si>
+    <t>client_user_id</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>profile_image_url</t>
+  </si>
+  <si>
+    <t>http://cloudinary.com/johndoe/profile.jpg</t>
+  </si>
+  <si>
+    <t>http://cloudinary.com/janedoe/profile.jpg</t>
+  </si>
+  <si>
+    <t>http://cloudinary.com/alicejohnson/profile.jpg</t>
+  </si>
+  <si>
+    <t>http://cloudinary.com/bobsmith/profile.jpg</t>
+  </si>
+  <si>
+    <t>bobsmith@example.com</t>
+  </si>
+  <si>
+    <t>alicejohnson@example.com</t>
+  </si>
+  <si>
+    <t>janedoe@example.com</t>
+  </si>
+  <si>
+    <t>johndoe@example.com</t>
+  </si>
+  <si>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>Johnson</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Jane</t>
+  </si>
+  <si>
+    <t>Alice</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>alicejohnson</t>
+  </si>
+  <si>
+    <t>bobsmith</t>
+  </si>
+  <si>
+    <t>johndoe</t>
+  </si>
+  <si>
+    <t>janedoe</t>
+  </si>
+  <si>
+    <t>clerk001</t>
+  </si>
+  <si>
+    <t>clerk002</t>
+  </si>
+  <si>
+    <t>clerk003</t>
+  </si>
+  <si>
+    <t>clerk004</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -69,8 +172,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -89,6 +206,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -99,18 +228,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -124,6 +258,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -391,8 +529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,4 +625,155 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ACC8885-22E2-406D-9572-C4689306DA77}">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="44" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="H3" r:id="rId1" xr:uid="{85CF1A53-80DF-4D01-8254-4137BAC83802}"/>
+    <hyperlink ref="H2" r:id="rId2" xr:uid="{B08099EF-B46C-4CA1-8C08-0758E2EBC558}"/>
+    <hyperlink ref="H4" r:id="rId3" xr:uid="{579945B0-B5C7-4116-8226-ECF6B4A50636}"/>
+    <hyperlink ref="H5" r:id="rId4" xr:uid="{2E3D650E-A1F6-46A8-BA07-FB2AD233BC0A}"/>
+    <hyperlink ref="F5" r:id="rId5" xr:uid="{E8904FA0-D033-4549-A687-6EAE2ACD73E7}"/>
+    <hyperlink ref="F4" r:id="rId6" xr:uid="{5FC297E7-605A-4E15-BBBE-F9CAC7E5554B}"/>
+    <hyperlink ref="F3" r:id="rId7" xr:uid="{3FF67404-933D-46AB-8432-23D0A794B66F}"/>
+    <hyperlink ref="F2" r:id="rId8" xr:uid="{D3CF61F4-A3C8-444A-8972-5C87BBCDB712}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>